<commit_message>
add further entries for solved
</commit_message>
<xml_diff>
--- a/TexasHoldemBonusSimulator/Assets/Texas_Holdem_Bonus_Solved.xlsx
+++ b/TexasHoldemBonusSimulator/Assets/Texas_Holdem_Bonus_Solved.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U56034\OWN_WS\BerldPokerEngine\TexasHoldemBonusSimulator\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EC0278-AE94-4D6B-8AA6-76EEBDD7101E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFAE226-E034-4759-A836-E0637BF7F741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD6B6ABC-476D-4D2B-8F01-A68FA1E46815}"/>
   </bookViews>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3F2A37-638D-40C7-9927-D8667CBDC363}">
   <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="I8" s="12">
         <f>SUM(G2:G170)</f>
-        <v>-12795429099760</v>
+        <v>-12793201867088</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="I11" s="11">
         <f>I8/I5</f>
-        <v>-0.23001935169469898</v>
+        <v>-0.2299793134426566</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3306,15 +3306,15 @@
         <v>4</v>
       </c>
       <c r="E92" s="12">
-        <v>0</v>
+        <v>556808168</v>
       </c>
       <c r="F92" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.3272680552051505E-2</v>
       </c>
       <c r="G92" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2227232672</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -5059,7 +5059,7 @@
         <v>0</v>
       </c>
       <c r="F162" s="11">
-        <f t="shared" ref="F162:F193" si="10">E162/$I$2</f>
+        <f t="shared" ref="F162:F170" si="10">E162/$I$2</f>
         <v>0</v>
       </c>
       <c r="G162" s="12">

</xml_diff>

<commit_message>
add texas holdem bonus solved progress
</commit_message>
<xml_diff>
--- a/TexasHoldemBonusSimulator/Assets/Texas_Holdem_Bonus_Solved.xlsx
+++ b/TexasHoldemBonusSimulator/Assets/Texas_Holdem_Bonus_Solved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U56034\OWN_WS\BerldPokerEngine\TexasHoldemBonusSimulator\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E65152-9C78-4793-B130-B8510535B95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC4A392-7405-4DA6-BF14-7FA6120C3F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD6B6ABC-476D-4D2B-8F01-A68FA1E46815}"/>
+    <workbookView xWindow="-28800" yWindow="2475" windowWidth="28800" windowHeight="15435" xr2:uid="{AD6B6ABC-476D-4D2B-8F01-A68FA1E46815}"/>
   </bookViews>
   <sheets>
     <sheet name="Winnings" sheetId="1" r:id="rId1"/>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3F2A37-638D-40C7-9927-D8667CBDC363}">
   <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="I8" s="12">
         <f>SUM(G2:G170)</f>
-        <v>-12333191584992</v>
+        <v>-12492725626008</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="I11" s="11">
         <f>I8/I5</f>
-        <v>-0.2217098551825501</v>
+        <v>-0.22457774780276898</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2531,15 +2531,15 @@
         <v>12</v>
       </c>
       <c r="E61" s="12">
-        <v>0</v>
+        <v>-9648241998</v>
       </c>
       <c r="F61" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-0.22998591128487389</v>
       </c>
       <c r="G61" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-115778903976</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2906,15 +2906,15 @@
         <v>12</v>
       </c>
       <c r="E76" s="12">
-        <v>0</v>
+        <v>-6618582004</v>
       </c>
       <c r="F76" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-0.15776766523053029</v>
       </c>
       <c r="G76" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-79422984048</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2931,15 +2931,15 @@
         <v>4</v>
       </c>
       <c r="E77" s="12">
-        <v>0</v>
+        <v>2780829246</v>
       </c>
       <c r="F77" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6.6286847738843246E-2</v>
       </c>
       <c r="G77" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>11123316984</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -3356,15 +3356,15 @@
         <v>4</v>
       </c>
       <c r="E94" s="12">
-        <v>0</v>
+        <v>6136132506</v>
       </c>
       <c r="F94" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.14626747820480476</v>
       </c>
       <c r="G94" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>24544530024</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add texas holdem bonus progress
</commit_message>
<xml_diff>
--- a/TexasHoldemBonusSimulator/Assets/Texas_Holdem_Bonus_Solved.xlsx
+++ b/TexasHoldemBonusSimulator/Assets/Texas_Holdem_Bonus_Solved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U56034\OWN_WS\BerldPokerEngine\TexasHoldemBonusSimulator\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC4A392-7405-4DA6-BF14-7FA6120C3F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10507D1C-593E-4E1C-8CBC-51D31D12557D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2475" windowWidth="28800" windowHeight="15435" xr2:uid="{AD6B6ABC-476D-4D2B-8F01-A68FA1E46815}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AD6B6ABC-476D-4D2B-8F01-A68FA1E46815}"/>
   </bookViews>
   <sheets>
     <sheet name="Winnings" sheetId="1" r:id="rId1"/>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3F2A37-638D-40C7-9927-D8667CBDC363}">
   <dimension ref="A1:I170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="I8" s="12">
         <f>SUM(G2:G170)</f>
-        <v>-12492725626008</v>
+        <v>-11947326213400</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="I11" s="11">
         <f>I8/I5</f>
-        <v>-0.22457774780276898</v>
+        <v>-0.2147732763524825</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -3331,15 +3331,15 @@
         <v>12</v>
       </c>
       <c r="E93" s="12">
-        <v>0</v>
+        <v>-3281278936</v>
       </c>
       <c r="F93" s="11">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-7.8216106771809166E-2</v>
       </c>
       <c r="G93" s="12">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-39375347232</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -3806,15 +3806,15 @@
         <v>12</v>
       </c>
       <c r="E112" s="12">
-        <v>0</v>
+        <v>834290640</v>
       </c>
       <c r="F112" s="11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.9887052289589622E-2</v>
       </c>
       <c r="G112" s="12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10011487680</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
@@ -3831,15 +3831,15 @@
         <v>4</v>
       </c>
       <c r="E113" s="12">
-        <v>0</v>
+        <v>10321042356</v>
       </c>
       <c r="F113" s="11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.24602350688824853</v>
       </c>
       <c r="G113" s="12">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>41284169424</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -4331,15 +4331,15 @@
         <v>12</v>
       </c>
       <c r="E133" s="12">
-        <v>0</v>
+        <v>9435360972</v>
       </c>
       <c r="F133" s="11">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.22491144934973401</v>
       </c>
       <c r="G133" s="12">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>113224331664</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -4356,15 +4356,15 @@
         <v>4</v>
       </c>
       <c r="E134" s="12">
-        <v>0</v>
+        <v>18924544432</v>
       </c>
       <c r="F134" s="11">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.45110586962337984</v>
       </c>
       <c r="G134" s="12">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>75698177728</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -4906,15 +4906,15 @@
         <v>12</v>
       </c>
       <c r="E156" s="12">
-        <v>0</v>
+        <v>19163347960</v>
       </c>
       <c r="F156" s="11">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.45679824829884297</v>
       </c>
       <c r="G156" s="12">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>229960175520</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.2">
@@ -4931,15 +4931,15 @@
         <v>4</v>
       </c>
       <c r="E157" s="12">
-        <v>0</v>
+        <v>28649104456</v>
       </c>
       <c r="F157" s="11">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>0.6829109797592684</v>
       </c>
       <c r="G157" s="12">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>114596417824</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>